<commit_message>
RDM-6436 -  added CallBackURLMidEvent url
</commit_message>
<xml_diff>
--- a/CCD_CNP_27_With_Callbacks.xlsx
+++ b/CCD_CNP_27_With_Callbacks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-test-stubs-service/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9343390-280C-174B-AAC6-6F29B34C5C62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F753B7E-18B8-D74D-8BCB-2BA6B0C794F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="28080" windowHeight="16620" tabRatio="823" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="28080" windowHeight="16620" tabRatio="823" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="288">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -910,6 +910,22 @@
   </si>
   <si>
     <t>http://localhost:5555/callback_submitted</t>
+  </si>
+  <si>
+    <t>URL to call back to the service for uniqueness. 
+Max Length: &lt;unlimited&gt;</t>
+  </si>
+  <si>
+    <t>CallBackURLMidEvent</t>
+  </si>
+  <si>
+    <t>DynamicList</t>
+  </si>
+  <si>
+    <t>A `DynamicList` field</t>
+  </si>
+  <si>
+    <t>http://localhost:5555/mid_event_dynamic_list</t>
   </si>
 </sst>
 </file>
@@ -921,7 +937,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1200,6 +1216,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1318,7 +1349,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1441,6 +1472,12 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2030,7 +2067,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$35</xm:f>
+            <xm:f>CaseField!$D$4:$D$36</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D7</xm:sqref>
         </x14:dataValidation>
@@ -2169,7 +2206,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0A00-000003000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$35</xm:f>
+            <xm:f>CaseField!$D$4:$D$36</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D5</xm:sqref>
         </x14:dataValidation>
@@ -2343,7 +2380,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000004000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$35</xm:f>
+            <xm:f>CaseField!$D$4:$D$36</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D7</xm:sqref>
         </x14:dataValidation>
@@ -4965,10 +5002,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5587,22 +5624,22 @@
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42" t="s">
         <v>26</v>
       </c>
       <c r="J21" s="28"/>
@@ -5619,16 +5656,16 @@
         <v>251</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28" t="s">
@@ -5648,16 +5685,16 @@
         <v>251</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="G23" s="42" t="s">
-        <v>30</v>
+        <v>142</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="28" t="s">
@@ -5676,17 +5713,17 @@
       <c r="C24" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="D24" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="F24" s="42" t="s">
-        <v>148</v>
+      <c r="D24" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="28" t="s">
@@ -5706,16 +5743,16 @@
         <v>251</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="H25" s="28"/>
       <c r="I25" s="28" t="s">
@@ -5735,16 +5772,16 @@
         <v>251</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G26" s="42" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28" t="s">
@@ -5764,16 +5801,16 @@
         <v>251</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G27" s="42" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
@@ -5793,16 +5830,16 @@
         <v>251</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>248</v>
+        <v>153</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>249</v>
+        <v>154</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>250</v>
+        <v>27</v>
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="28" t="s">
@@ -5822,16 +5859,16 @@
         <v>251</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>157</v>
+        <v>248</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>159</v>
+        <v>249</v>
       </c>
       <c r="G29" s="42" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28" t="s">
@@ -5851,20 +5888,18 @@
         <v>251</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G30" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="42" t="s">
-        <v>163</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="H30" s="28"/>
       <c r="I30" s="28" t="s">
         <v>26</v>
       </c>
@@ -5882,19 +5917,19 @@
         <v>251</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F31" s="42" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G31" s="42" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="I31" s="28" t="s">
         <v>26</v>
@@ -5913,19 +5948,19 @@
         <v>251</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>240</v>
+        <v>170</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="F32" s="42" t="s">
-        <v>242</v>
+        <v>172</v>
       </c>
       <c r="G32" s="42" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="H32" s="42" t="s">
-        <v>25</v>
+        <v>173</v>
       </c>
       <c r="I32" s="28" t="s">
         <v>26</v>
@@ -5944,18 +5979,20 @@
         <v>251</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="F33" s="42" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="G33" s="42" t="s">
-        <v>228</v>
-      </c>
-      <c r="H33" s="42"/>
+        <v>80</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>25</v>
+      </c>
       <c r="I33" s="28" t="s">
         <v>26</v>
       </c>
@@ -5973,16 +6010,16 @@
         <v>251</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="F34" s="42" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="G34" s="42" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="H34" s="42"/>
       <c r="I34" s="28" t="s">
@@ -6002,20 +6039,18 @@
         <v>251</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="F35" s="42" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="G35" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="H35" s="42" t="s">
-        <v>262</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="H35" s="42"/>
       <c r="I35" s="28" t="s">
         <v>26</v>
       </c>
@@ -6033,18 +6068,20 @@
         <v>251</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>271</v>
-      </c>
-      <c r="G36" s="75" t="s">
-        <v>272</v>
-      </c>
-      <c r="H36" s="42"/>
+        <v>260</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>262</v>
+      </c>
       <c r="I36" s="28" t="s">
         <v>26</v>
       </c>
@@ -6053,12 +6090,41 @@
         <v>117</v>
       </c>
     </row>
+    <row r="37" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="F37" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="G37" s="75" t="s">
+        <v>272</v>
+      </c>
+      <c r="H37" s="42"/>
+      <c r="I37" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A37" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B36" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B37" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -6820,8 +6886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7436,10 +7502,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O91"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView topLeftCell="L2" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7458,9 +7524,10 @@
     <col min="13" max="13" width="28.6640625" customWidth="1"/>
     <col min="14" max="14" width="28.6640625" style="14" customWidth="1"/>
     <col min="15" max="15" width="23.33203125" customWidth="1"/>
+    <col min="16" max="16" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -7481,7 +7548,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:15" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43" t="s">
@@ -7523,8 +7590,11 @@
       <c r="O2" s="46" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P2" s="88" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -7570,8 +7640,11 @@
       <c r="O3" s="45" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P3" s="89" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -7608,7 +7681,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -7645,7 +7718,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -7682,7 +7755,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -7719,7 +7792,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -7756,7 +7829,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -7793,7 +7866,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -7830,7 +7903,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -7867,7 +7940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -7904,7 +7977,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -7941,7 +8014,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -7978,7 +8051,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -8015,7 +8088,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13">
         <v>42736</v>
       </c>
@@ -8052,7 +8125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13">
         <v>42736</v>
       </c>
@@ -8089,7 +8162,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>42736</v>
       </c>
@@ -8126,7 +8199,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>42736</v>
       </c>
@@ -8163,7 +8236,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13">
         <v>42736</v>
       </c>
@@ -8172,13 +8245,13 @@
         <v>234</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>135</v>
+        <v>190</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>285</v>
       </c>
       <c r="F20" s="28">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="42" t="s">
@@ -8188,19 +8261,22 @@
         <v>201</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="L20" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O20" s="24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P20" s="73" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13">
         <v>42736</v>
       </c>
@@ -8212,10 +8288,10 @@
         <v>198</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F21" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="28"/>
       <c r="H21" s="42" t="s">
@@ -8237,7 +8313,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13">
         <v>42736</v>
       </c>
@@ -8249,10 +8325,10 @@
         <v>198</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F22" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="42" t="s">
@@ -8274,7 +8350,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>42736</v>
       </c>
@@ -8285,11 +8361,11 @@
       <c r="D23" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="E23" s="42" t="s">
-        <v>144</v>
+      <c r="E23" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="F23" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="42" t="s">
@@ -8311,7 +8387,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>42736</v>
       </c>
@@ -8323,10 +8399,10 @@
         <v>198</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F24" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="42" t="s">
@@ -8348,7 +8424,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>42736</v>
       </c>
@@ -8360,10 +8436,10 @@
         <v>198</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F25" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G25" s="28"/>
       <c r="H25" s="42" t="s">
@@ -8373,19 +8449,19 @@
         <v>201</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L25" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O25" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>42736</v>
       </c>
@@ -8397,10 +8473,10 @@
         <v>198</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F26" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="28"/>
       <c r="H26" s="42" t="s">
@@ -8422,7 +8498,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>42736</v>
       </c>
@@ -8434,10 +8510,10 @@
         <v>198</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="F27" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27" s="28"/>
       <c r="H27" s="42" t="s">
@@ -8459,7 +8535,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>42736</v>
       </c>
@@ -8471,10 +8547,10 @@
         <v>198</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="F28" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G28" s="28"/>
       <c r="H28" s="42" t="s">
@@ -8496,7 +8572,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>42736</v>
       </c>
@@ -8508,10 +8584,10 @@
         <v>198</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F29" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G29" s="28"/>
       <c r="H29" s="42" t="s">
@@ -8533,7 +8609,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>42736</v>
       </c>
@@ -8545,10 +8621,10 @@
         <v>198</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F30" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G30" s="28"/>
       <c r="H30" s="42" t="s">
@@ -8570,7 +8646,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13">
         <v>42736</v>
       </c>
@@ -8582,10 +8658,10 @@
         <v>198</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="F31" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G31" s="28"/>
       <c r="H31" s="42" t="s">
@@ -8595,19 +8671,19 @@
         <v>201</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="K31" s="24" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="L31" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O31" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>42736</v>
       </c>
@@ -8619,10 +8695,10 @@
         <v>198</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="F32" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" s="28"/>
       <c r="H32" s="42" t="s">
@@ -8656,10 +8732,10 @@
         <v>198</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F33" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G33" s="28"/>
       <c r="H33" s="42" t="s">
@@ -8693,10 +8769,10 @@
         <v>198</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="F34" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G34" s="28"/>
       <c r="H34" s="42" t="s">
@@ -8715,7 +8791,7 @@
         <v>3</v>
       </c>
       <c r="O34" s="24" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8727,32 +8803,32 @@
         <v>234</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>206</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>135</v>
+        <v>198</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>254</v>
       </c>
       <c r="F35" s="28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G35" s="28"/>
-      <c r="H35" s="28" t="s">
-        <v>73</v>
+      <c r="H35" s="42" t="s">
+        <v>26</v>
       </c>
       <c r="I35" s="28" t="s">
         <v>201</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="K35" s="24" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="L35" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O35" s="24" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8767,10 +8843,10 @@
         <v>206</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F36" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="28" t="s">
@@ -8804,10 +8880,10 @@
         <v>206</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F37" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="28" t="s">
@@ -8840,11 +8916,11 @@
       <c r="D38" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="E38" s="42" t="s">
-        <v>144</v>
+      <c r="E38" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="F38" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="28" t="s">
@@ -8878,10 +8954,10 @@
         <v>206</v>
       </c>
       <c r="E39" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F39" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="28" t="s">
@@ -8915,10 +8991,10 @@
         <v>206</v>
       </c>
       <c r="E40" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F40" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="28" t="s">
@@ -8928,13 +9004,13 @@
         <v>201</v>
       </c>
       <c r="J40" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K40" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L40" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O40" s="24" t="s">
         <v>26</v>
@@ -8952,10 +9028,10 @@
         <v>206</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F41" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" s="28"/>
       <c r="H41" s="28" t="s">
@@ -8989,10 +9065,10 @@
         <v>206</v>
       </c>
       <c r="E42" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="F42" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="28" t="s">
@@ -9026,10 +9102,10 @@
         <v>206</v>
       </c>
       <c r="E43" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="F43" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G43" s="28"/>
       <c r="H43" s="28" t="s">
@@ -9063,10 +9139,10 @@
         <v>206</v>
       </c>
       <c r="E44" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F44" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G44" s="28"/>
       <c r="H44" s="28" t="s">
@@ -9100,10 +9176,10 @@
         <v>206</v>
       </c>
       <c r="E45" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F45" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G45" s="28"/>
       <c r="H45" s="28" t="s">
@@ -9137,10 +9213,10 @@
         <v>206</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="F46" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G46" s="28"/>
       <c r="H46" s="28" t="s">
@@ -9150,13 +9226,13 @@
         <v>201</v>
       </c>
       <c r="J46" s="24" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="K46" s="24" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="L46" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O46" s="24" t="s">
         <v>26</v>
@@ -9174,10 +9250,10 @@
         <v>206</v>
       </c>
       <c r="E47" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="F47" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" s="28"/>
       <c r="H47" s="28" t="s">
@@ -9211,10 +9287,10 @@
         <v>206</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F48" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G48" s="28"/>
       <c r="H48" s="28" t="s">
@@ -9242,35 +9318,35 @@
       </c>
       <c r="B49" s="13"/>
       <c r="C49" s="14" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>190</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>135</v>
+        <v>206</v>
+      </c>
+      <c r="E49" s="42" t="s">
+        <v>243</v>
       </c>
       <c r="F49" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G49" s="28"/>
-      <c r="H49" s="42" t="s">
-        <v>26</v>
+      <c r="H49" s="28" t="s">
+        <v>73</v>
       </c>
       <c r="I49" s="28" t="s">
         <v>201</v>
       </c>
       <c r="J49" s="24" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="K49" s="24" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="L49" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O49" s="24" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9285,10 +9361,10 @@
         <v>190</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F50" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G50" s="28"/>
       <c r="H50" s="42" t="s">
@@ -9322,10 +9398,10 @@
         <v>190</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F51" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G51" s="28"/>
       <c r="H51" s="42" t="s">
@@ -9358,11 +9434,11 @@
       <c r="D52" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="E52" s="42" t="s">
-        <v>144</v>
+      <c r="E52" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="F52" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G52" s="28"/>
       <c r="H52" s="42" t="s">
@@ -9396,10 +9472,10 @@
         <v>190</v>
       </c>
       <c r="E53" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F53" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G53" s="28"/>
       <c r="H53" s="42" t="s">
@@ -9433,10 +9509,10 @@
         <v>190</v>
       </c>
       <c r="E54" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F54" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="42" t="s">
@@ -9446,13 +9522,13 @@
         <v>201</v>
       </c>
       <c r="J54" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K54" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L54" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O54" s="24" t="s">
         <v>73</v>
@@ -9470,10 +9546,10 @@
         <v>190</v>
       </c>
       <c r="E55" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F55" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G55" s="28"/>
       <c r="H55" s="42" t="s">
@@ -9507,10 +9583,10 @@
         <v>190</v>
       </c>
       <c r="E56" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="F56" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G56" s="28"/>
       <c r="H56" s="42" t="s">
@@ -9544,10 +9620,10 @@
         <v>190</v>
       </c>
       <c r="E57" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="F57" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G57" s="28"/>
       <c r="H57" s="42" t="s">
@@ -9581,10 +9657,10 @@
         <v>190</v>
       </c>
       <c r="E58" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F58" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G58" s="28"/>
       <c r="H58" s="42" t="s">
@@ -9618,10 +9694,10 @@
         <v>190</v>
       </c>
       <c r="E59" s="42" t="s">
-        <v>258</v>
+        <v>160</v>
       </c>
       <c r="F59" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G59" s="28"/>
       <c r="H59" s="42" t="s">
@@ -9655,10 +9731,10 @@
         <v>190</v>
       </c>
       <c r="E60" s="42" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="F60" s="28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G60" s="28"/>
       <c r="H60" s="42" t="s">
@@ -9692,10 +9768,10 @@
         <v>190</v>
       </c>
       <c r="E61" s="42" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="F61" s="28">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G61" s="28"/>
       <c r="H61" s="42" t="s">
@@ -9705,16 +9781,16 @@
         <v>201</v>
       </c>
       <c r="J61" s="24" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="K61" s="24" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="L61" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O61" s="24" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9729,10 +9805,10 @@
         <v>190</v>
       </c>
       <c r="E62" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="F62" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G62" s="28"/>
       <c r="H62" s="42" t="s">
@@ -9766,10 +9842,10 @@
         <v>190</v>
       </c>
       <c r="E63" s="42" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F63" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G63" s="28"/>
       <c r="H63" s="42" t="s">
@@ -9800,13 +9876,13 @@
         <v>251</v>
       </c>
       <c r="D64" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="E64" s="28" t="s">
-        <v>135</v>
+        <v>190</v>
+      </c>
+      <c r="E64" s="42" t="s">
+        <v>243</v>
       </c>
       <c r="F64" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G64" s="28"/>
       <c r="H64" s="42" t="s">
@@ -9816,16 +9892,16 @@
         <v>201</v>
       </c>
       <c r="J64" s="24" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="K64" s="24" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="L64" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O64" s="24" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9840,10 +9916,10 @@
         <v>198</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F65" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G65" s="28"/>
       <c r="H65" s="42" t="s">
@@ -9877,10 +9953,10 @@
         <v>198</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F66" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G66" s="28"/>
       <c r="H66" s="42" t="s">
@@ -9913,11 +9989,11 @@
       <c r="D67" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="E67" s="42" t="s">
-        <v>144</v>
+      <c r="E67" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="F67" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G67" s="28"/>
       <c r="H67" s="42" t="s">
@@ -9951,10 +10027,10 @@
         <v>198</v>
       </c>
       <c r="E68" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F68" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G68" s="28"/>
       <c r="H68" s="42" t="s">
@@ -9988,10 +10064,10 @@
         <v>198</v>
       </c>
       <c r="E69" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F69" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G69" s="28"/>
       <c r="H69" s="42" t="s">
@@ -10001,13 +10077,13 @@
         <v>201</v>
       </c>
       <c r="J69" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K69" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L69" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O69" s="24" t="s">
         <v>73</v>
@@ -10025,10 +10101,10 @@
         <v>198</v>
       </c>
       <c r="E70" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F70" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G70" s="28"/>
       <c r="H70" s="42" t="s">
@@ -10062,10 +10138,10 @@
         <v>198</v>
       </c>
       <c r="E71" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="F71" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G71" s="28"/>
       <c r="H71" s="42" t="s">
@@ -10099,10 +10175,10 @@
         <v>198</v>
       </c>
       <c r="E72" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="F72" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G72" s="28"/>
       <c r="H72" s="42" t="s">
@@ -10136,10 +10212,10 @@
         <v>198</v>
       </c>
       <c r="E73" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F73" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G73" s="28"/>
       <c r="H73" s="42" t="s">
@@ -10173,10 +10249,10 @@
         <v>198</v>
       </c>
       <c r="E74" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F74" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G74" s="28"/>
       <c r="H74" s="42" t="s">
@@ -10210,10 +10286,10 @@
         <v>198</v>
       </c>
       <c r="E75" s="42" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="F75" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G75" s="28"/>
       <c r="H75" s="42" t="s">
@@ -10223,16 +10299,16 @@
         <v>201</v>
       </c>
       <c r="J75" s="24" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="K75" s="24" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="L75" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O75" s="24" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10247,10 +10323,10 @@
         <v>198</v>
       </c>
       <c r="E76" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="F76" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G76" s="28"/>
       <c r="H76" s="42" t="s">
@@ -10284,10 +10360,10 @@
         <v>198</v>
       </c>
       <c r="E77" s="42" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F77" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G77" s="28"/>
       <c r="H77" s="42" t="s">
@@ -10318,29 +10394,29 @@
         <v>251</v>
       </c>
       <c r="D78" s="42" t="s">
-        <v>206</v>
-      </c>
-      <c r="E78" s="28" t="s">
-        <v>135</v>
+        <v>198</v>
+      </c>
+      <c r="E78" s="42" t="s">
+        <v>243</v>
       </c>
       <c r="F78" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G78" s="28"/>
-      <c r="H78" s="28" t="s">
-        <v>73</v>
+      <c r="H78" s="42" t="s">
+        <v>26</v>
       </c>
       <c r="I78" s="28" t="s">
         <v>201</v>
       </c>
       <c r="J78" s="24" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="K78" s="24" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="L78" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O78" s="24" t="s">
         <v>26</v>
@@ -10358,10 +10434,10 @@
         <v>206</v>
       </c>
       <c r="E79" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F79" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G79" s="28"/>
       <c r="H79" s="28" t="s">
@@ -10395,10 +10471,10 @@
         <v>206</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F80" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G80" s="28"/>
       <c r="H80" s="28" t="s">
@@ -10431,11 +10507,11 @@
       <c r="D81" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="E81" s="42" t="s">
-        <v>144</v>
+      <c r="E81" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="F81" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G81" s="28"/>
       <c r="H81" s="28" t="s">
@@ -10469,10 +10545,10 @@
         <v>206</v>
       </c>
       <c r="E82" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F82" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G82" s="28"/>
       <c r="H82" s="28" t="s">
@@ -10506,10 +10582,10 @@
         <v>206</v>
       </c>
       <c r="E83" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F83" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G83" s="28"/>
       <c r="H83" s="28" t="s">
@@ -10519,13 +10595,13 @@
         <v>201</v>
       </c>
       <c r="J83" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K83" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L83" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O83" s="24" t="s">
         <v>26</v>
@@ -10543,10 +10619,10 @@
         <v>206</v>
       </c>
       <c r="E84" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F84" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G84" s="28"/>
       <c r="H84" s="28" t="s">
@@ -10580,10 +10656,10 @@
         <v>206</v>
       </c>
       <c r="E85" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="F85" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G85" s="28"/>
       <c r="H85" s="28" t="s">
@@ -10617,10 +10693,10 @@
         <v>206</v>
       </c>
       <c r="E86" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="F86" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G86" s="28"/>
       <c r="H86" s="28" t="s">
@@ -10654,10 +10730,10 @@
         <v>206</v>
       </c>
       <c r="E87" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F87" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G87" s="28"/>
       <c r="H87" s="28" t="s">
@@ -10691,10 +10767,10 @@
         <v>206</v>
       </c>
       <c r="E88" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F88" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G88" s="28"/>
       <c r="H88" s="28" t="s">
@@ -10728,10 +10804,10 @@
         <v>206</v>
       </c>
       <c r="E89" s="42" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="F89" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G89" s="28"/>
       <c r="H89" s="28" t="s">
@@ -10741,13 +10817,13 @@
         <v>201</v>
       </c>
       <c r="J89" s="24" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="K89" s="24" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="L89" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O89" s="24" t="s">
         <v>26</v>
@@ -10765,10 +10841,10 @@
         <v>206</v>
       </c>
       <c r="E90" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="F90" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G90" s="28"/>
       <c r="H90" s="28" t="s">
@@ -10802,10 +10878,10 @@
         <v>206</v>
       </c>
       <c r="E91" s="42" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F91" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G91" s="28"/>
       <c r="H91" s="28" t="s">
@@ -10827,15 +10903,55 @@
         <v>26</v>
       </c>
     </row>
+    <row r="92" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B92" s="13"/>
+      <c r="C92" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D92" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="E92" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="F92" s="28">
+        <v>3</v>
+      </c>
+      <c r="G92" s="28"/>
+      <c r="H92" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I92" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="J92" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="K92" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="L92" s="14">
+        <v>3</v>
+      </c>
+      <c r="O92" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A20:A91 A4:A19" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A92" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B20:B91 B4:B19" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B92" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="P20" r:id="rId1" xr:uid="{77676679-8B66-5049-945F-8500F2701C4F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -10971,7 +11087,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$35</xm:f>
+            <xm:f>CaseField!$D$4:$D$36</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D5</xm:sqref>
         </x14:dataValidation>

</xml_diff>